<commit_message>
Updated test cases and marked execution mode of them.
</commit_message>
<xml_diff>
--- a/TestCases/Create Appointment Tests.xlsx
+++ b/TestCases/Create Appointment Tests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>2. The applicant should see an error message that tells them that they are unable to schedule an appointment in that timeslot because it is full.</t>
+  </si>
+  <si>
+    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +565,9 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -576,6 +582,9 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -590,6 +599,9 @@
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -604,6 +616,9 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -618,6 +633,9 @@
       <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -631,6 +649,9 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>